<commit_message>
Add regionally extinct (RE) as a red list category
REQUEST: France: in Kobo Section 8, for the national Red List assessments, consider adding category “RE”, regionally extinct.

CHANGE DONE:
select_one ce5ds76	regional_redlist	National Red List Category
</commit_message>
<xml_diff>
--- a/kobo_form.xlsx
+++ b/kobo_form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ticatla/Science/CONABIO/CBD Gen Div/Kobo_forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D634DF4B-34E2-3A4E-A466-259DE1D54AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D90D96B-EE86-B941-846A-9145C69157B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="22140" windowHeight="15360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5395" uniqueCount="2357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5398" uniqueCount="2359">
   <si>
     <t>type</t>
   </si>
@@ -7093,6 +7093,12 @@
   </si>
   <si>
     <t>${n_extant_populations} &gt; 25</t>
+  </si>
+  <si>
+    <t>re</t>
+  </si>
+  <si>
+    <t>Regionally extinct (RE). Select only for National Redlists.</t>
   </si>
 </sst>
 </file>
@@ -7470,12 +7476,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L686"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A665" workbookViewId="0">
+      <selection activeCell="A663" sqref="A663:C663"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="54.83203125" customWidth="1"/>
   </cols>
@@ -21630,10 +21637,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D353"/>
+  <dimension ref="A1:D354"/>
   <sheetViews>
-    <sheetView topLeftCell="A237" workbookViewId="0">
-      <selection activeCell="C251" sqref="C251"/>
+    <sheetView topLeftCell="A377" workbookViewId="0">
+      <selection activeCell="D304" sqref="D304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -25226,13 +25233,13 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>2271</v>
+        <v>2256</v>
       </c>
       <c r="B315" t="s">
-        <v>2272</v>
+        <v>2357</v>
       </c>
       <c r="C315" t="s">
-        <v>2273</v>
+        <v>2358</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
@@ -25240,13 +25247,10 @@
         <v>2271</v>
       </c>
       <c r="B316" t="s">
-        <v>2274</v>
+        <v>2272</v>
       </c>
       <c r="C316" t="s">
-        <v>2275</v>
-      </c>
-      <c r="D316" t="s">
-        <v>2042</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="317" spans="1:4" x14ac:dyDescent="0.2">
@@ -25254,13 +25258,13 @@
         <v>2271</v>
       </c>
       <c r="B317" t="s">
-        <v>2276</v>
+        <v>2274</v>
       </c>
       <c r="C317" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="D317" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="318" spans="1:4" x14ac:dyDescent="0.2">
@@ -25268,13 +25272,13 @@
         <v>2271</v>
       </c>
       <c r="B318" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="C318" t="s">
-        <v>2278</v>
+        <v>2276</v>
       </c>
       <c r="D318" t="s">
-        <v>2051</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="319" spans="1:4" x14ac:dyDescent="0.2">
@@ -25282,13 +25286,13 @@
         <v>2271</v>
       </c>
       <c r="B319" t="s">
-        <v>2279</v>
+        <v>2277</v>
       </c>
       <c r="C319" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="D319" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="320" spans="1:4" x14ac:dyDescent="0.2">
@@ -25296,13 +25300,13 @@
         <v>2271</v>
       </c>
       <c r="B320" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="C320" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="D320" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.2">
@@ -25310,13 +25314,13 @@
         <v>2271</v>
       </c>
       <c r="B321" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="C321" t="s">
-        <v>2282</v>
+        <v>2280</v>
       </c>
       <c r="D321" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.2">
@@ -25324,13 +25328,13 @@
         <v>2271</v>
       </c>
       <c r="B322" t="s">
-        <v>2283</v>
+        <v>2281</v>
       </c>
       <c r="C322" t="s">
-        <v>2284</v>
+        <v>2282</v>
       </c>
       <c r="D322" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.2">
@@ -25338,13 +25342,13 @@
         <v>2271</v>
       </c>
       <c r="B323" t="s">
-        <v>2285</v>
+        <v>2283</v>
       </c>
       <c r="C323" t="s">
-        <v>2286</v>
+        <v>2284</v>
       </c>
       <c r="D323" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.2">
@@ -25352,13 +25356,13 @@
         <v>2271</v>
       </c>
       <c r="B324" t="s">
-        <v>2287</v>
+        <v>2285</v>
       </c>
       <c r="C324" t="s">
-        <v>2288</v>
+        <v>2286</v>
       </c>
       <c r="D324" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.2">
@@ -25366,13 +25370,13 @@
         <v>2271</v>
       </c>
       <c r="B325" t="s">
-        <v>2289</v>
+        <v>2287</v>
       </c>
       <c r="C325" t="s">
-        <v>2079</v>
+        <v>2288</v>
       </c>
       <c r="D325" t="s">
-        <v>2072</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.2">
@@ -25380,24 +25384,27 @@
         <v>2271</v>
       </c>
       <c r="B326" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="C326" t="s">
-        <v>2291</v>
+        <v>2079</v>
       </c>
       <c r="D326" t="s">
-        <v>2210</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>2292</v>
+        <v>2271</v>
       </c>
       <c r="B327" t="s">
-        <v>2293</v>
+        <v>2290</v>
       </c>
       <c r="C327" t="s">
-        <v>2294</v>
+        <v>2291</v>
+      </c>
+      <c r="D327" t="s">
+        <v>2210</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.2">
@@ -25405,13 +25412,10 @@
         <v>2292</v>
       </c>
       <c r="B328" t="s">
-        <v>2295</v>
+        <v>2293</v>
       </c>
       <c r="C328" t="s">
-        <v>2296</v>
-      </c>
-      <c r="D328" t="s">
-        <v>2042</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.2">
@@ -25419,13 +25423,13 @@
         <v>2292</v>
       </c>
       <c r="B329" t="s">
-        <v>2297</v>
+        <v>2295</v>
       </c>
       <c r="C329" t="s">
-        <v>2298</v>
+        <v>2296</v>
       </c>
       <c r="D329" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.2">
@@ -25433,13 +25437,13 @@
         <v>2292</v>
       </c>
       <c r="B330" t="s">
-        <v>2299</v>
+        <v>2297</v>
       </c>
       <c r="C330" t="s">
-        <v>2300</v>
+        <v>2298</v>
       </c>
       <c r="D330" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.2">
@@ -25447,13 +25451,13 @@
         <v>2292</v>
       </c>
       <c r="B331" t="s">
-        <v>2301</v>
+        <v>2299</v>
       </c>
       <c r="C331" t="s">
-        <v>2302</v>
+        <v>2300</v>
       </c>
       <c r="D331" t="s">
-        <v>2051</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.2">
@@ -25461,13 +25465,13 @@
         <v>2292</v>
       </c>
       <c r="B332" t="s">
-        <v>2303</v>
+        <v>2301</v>
       </c>
       <c r="C332" t="s">
-        <v>2304</v>
+        <v>2302</v>
       </c>
       <c r="D332" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.2">
@@ -25475,13 +25479,13 @@
         <v>2292</v>
       </c>
       <c r="B333" t="s">
-        <v>2305</v>
+        <v>2303</v>
       </c>
       <c r="C333" t="s">
-        <v>2306</v>
+        <v>2304</v>
       </c>
       <c r="D333" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.2">
@@ -25489,13 +25493,13 @@
         <v>2292</v>
       </c>
       <c r="B334" t="s">
-        <v>2307</v>
+        <v>2305</v>
       </c>
       <c r="C334" t="s">
-        <v>2308</v>
+        <v>2306</v>
       </c>
       <c r="D334" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.2">
@@ -25503,13 +25507,13 @@
         <v>2292</v>
       </c>
       <c r="B335" t="s">
-        <v>2309</v>
+        <v>2307</v>
       </c>
       <c r="C335" t="s">
-        <v>2310</v>
+        <v>2308</v>
       </c>
       <c r="D335" t="s">
-        <v>2063</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.2">
@@ -25517,13 +25521,13 @@
         <v>2292</v>
       </c>
       <c r="B336" t="s">
-        <v>2311</v>
+        <v>2309</v>
       </c>
       <c r="C336" t="s">
-        <v>2312</v>
+        <v>2310</v>
       </c>
       <c r="D336" t="s">
-        <v>2066</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.2">
@@ -25531,13 +25535,13 @@
         <v>2292</v>
       </c>
       <c r="B337" t="s">
-        <v>2070</v>
+        <v>2311</v>
       </c>
       <c r="C337" t="s">
-        <v>2071</v>
+        <v>2312</v>
       </c>
       <c r="D337" t="s">
-        <v>2069</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.2">
@@ -25545,21 +25549,24 @@
         <v>2292</v>
       </c>
       <c r="B338" t="s">
-        <v>2078</v>
+        <v>2070</v>
       </c>
       <c r="C338" t="s">
-        <v>2079</v>
+        <v>2071</v>
+      </c>
+      <c r="D338" t="s">
+        <v>2069</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>2313</v>
+        <v>2292</v>
       </c>
       <c r="B339" t="s">
-        <v>2314</v>
+        <v>2078</v>
       </c>
       <c r="C339" t="s">
-        <v>2315</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.2">
@@ -25567,10 +25574,10 @@
         <v>2313</v>
       </c>
       <c r="B340" t="s">
-        <v>2316</v>
+        <v>2314</v>
       </c>
       <c r="C340" t="s">
-        <v>2317</v>
+        <v>2315</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.2">
@@ -25578,10 +25585,10 @@
         <v>2313</v>
       </c>
       <c r="B341" t="s">
-        <v>2318</v>
+        <v>2316</v>
       </c>
       <c r="C341" t="s">
-        <v>2319</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.2">
@@ -25589,10 +25596,10 @@
         <v>2313</v>
       </c>
       <c r="B342" t="s">
-        <v>2070</v>
+        <v>2318</v>
       </c>
       <c r="C342" t="s">
-        <v>2071</v>
+        <v>2319</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.2">
@@ -25600,21 +25607,21 @@
         <v>2313</v>
       </c>
       <c r="B343" t="s">
-        <v>2078</v>
+        <v>2070</v>
       </c>
       <c r="C343" t="s">
-        <v>2079</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>2320</v>
+        <v>2313</v>
       </c>
       <c r="B344" t="s">
-        <v>2321</v>
+        <v>2078</v>
       </c>
       <c r="C344" t="s">
-        <v>2322</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.2">
@@ -25622,13 +25629,10 @@
         <v>2320</v>
       </c>
       <c r="B345" t="s">
-        <v>2323</v>
+        <v>2321</v>
       </c>
       <c r="C345" t="s">
-        <v>2324</v>
-      </c>
-      <c r="D345" t="s">
-        <v>2042</v>
+        <v>2322</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.2">
@@ -25636,13 +25640,13 @@
         <v>2320</v>
       </c>
       <c r="B346" t="s">
-        <v>2325</v>
+        <v>2323</v>
       </c>
       <c r="C346" t="s">
-        <v>2326</v>
+        <v>2324</v>
       </c>
       <c r="D346" t="s">
-        <v>2045</v>
+        <v>2042</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.2">
@@ -25650,13 +25654,13 @@
         <v>2320</v>
       </c>
       <c r="B347" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="C347" t="s">
-        <v>2328</v>
+        <v>2326</v>
       </c>
       <c r="D347" t="s">
-        <v>2048</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.2">
@@ -25664,13 +25668,13 @@
         <v>2320</v>
       </c>
       <c r="B348" t="s">
-        <v>2329</v>
+        <v>2327</v>
       </c>
       <c r="C348" t="s">
-        <v>2330</v>
+        <v>2328</v>
       </c>
       <c r="D348" t="s">
-        <v>2051</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.2">
@@ -25678,13 +25682,13 @@
         <v>2320</v>
       </c>
       <c r="B349" t="s">
-        <v>2331</v>
+        <v>2329</v>
       </c>
       <c r="C349" t="s">
-        <v>2332</v>
+        <v>2330</v>
       </c>
       <c r="D349" t="s">
-        <v>2054</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.2">
@@ -25692,13 +25696,13 @@
         <v>2320</v>
       </c>
       <c r="B350" t="s">
-        <v>2333</v>
+        <v>2331</v>
       </c>
       <c r="C350" t="s">
-        <v>2334</v>
+        <v>2332</v>
       </c>
       <c r="D350" t="s">
-        <v>2057</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.2">
@@ -25706,24 +25710,27 @@
         <v>2320</v>
       </c>
       <c r="B351" t="s">
-        <v>2078</v>
+        <v>2333</v>
       </c>
       <c r="C351" t="s">
-        <v>2079</v>
+        <v>2334</v>
       </c>
       <c r="D351" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>2335</v>
+        <v>2320</v>
       </c>
       <c r="B352" t="s">
-        <v>2336</v>
+        <v>2078</v>
       </c>
       <c r="C352" t="s">
-        <v>2337</v>
+        <v>2079</v>
+      </c>
+      <c r="D352" t="s">
+        <v>2060</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
@@ -25731,9 +25738,20 @@
         <v>2335</v>
       </c>
       <c r="B353" t="s">
+        <v>2336</v>
+      </c>
+      <c r="C353" t="s">
+        <v>2337</v>
+      </c>
+    </row>
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A354" t="s">
+        <v>2335</v>
+      </c>
+      <c r="B354" t="s">
         <v>2338</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C354" t="s">
         <v>2339</v>
       </c>
     </row>

</xml_diff>